<commit_message>
Edición antes de corrección de estilo tema 2
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion02/SolicitudGrafica-MA_11_02_CO_REC150.xlsx
+++ b/fuentes/contenidos/grado11/guion02/SolicitudGrafica-MA_11_02_CO_REC150.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="182">
   <si>
     <t>Fecha:</t>
   </si>
@@ -549,15 +549,9 @@
     <t>IMG09</t>
   </si>
   <si>
-    <t>Representacion grafica de la funcion f(x)=2^x</t>
-  </si>
-  <si>
     <t>IMG10</t>
   </si>
   <si>
-    <t>grafica de f(x)=ln(x)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -570,135 +564,61 @@
     <t>Gráfica de la funcion constante f(x)=4</t>
   </si>
   <si>
-    <t>Gráfica de la funcion constante f(x)=1/2</t>
-  </si>
-  <si>
     <t>Gráfica de la funcion constante f(x)=-2</t>
   </si>
   <si>
     <t>Grafica de la funcion f(x)=-2x</t>
   </si>
   <si>
-    <t>Grafica de la funcion f(x)=3x</t>
-  </si>
-  <si>
     <t>Grafica de la funcion f(x)=(-1/2)x</t>
   </si>
   <si>
-    <t>Grafica de la fncion f(x)=12x</t>
-  </si>
-  <si>
-    <t>Grafica de la funcion f(x)=8x</t>
-  </si>
-  <si>
-    <t>Grafica de la funcion f(x)=-8x</t>
-  </si>
-  <si>
-    <t>Grafica de la funcion f(x)=-12x</t>
-  </si>
-  <si>
-    <t>Grafica de la funcion f(x)=(-1/4)x</t>
-  </si>
-  <si>
     <t>Grafica de la función f(x)=-(1/10)x+4</t>
   </si>
   <si>
-    <t>Grafica de la funcion f(x)=-3x+4</t>
-  </si>
-  <si>
-    <t>Grafica de la funcion f(x)=x+1</t>
-  </si>
-  <si>
-    <t>Grafica de la funcion f(x)=-6x+2</t>
-  </si>
-  <si>
-    <t>Grafica de la función f(x)=-3x-1</t>
-  </si>
-  <si>
-    <t>Grafica de la funcion f(x)=(-1/3)x-2</t>
-  </si>
-  <si>
-    <r>
-      <t>Representacion grafica de la funcion f(x)=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>0.25x^6-1.5x^4+0.4x^2-0.45x-0.2</t>
-    </r>
-  </si>
-  <si>
-    <t>Representacion grafica de la función f(x)=x^2-x-1</t>
-  </si>
-  <si>
-    <r>
-      <t>Representación gráfica de la función f(x)=x</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>-4</t>
-    </r>
-  </si>
-  <si>
-    <t>Representacion grafica de la función f(x)=x^2-x+2</t>
-  </si>
-  <si>
-    <t>Representacion grafica de la función f(x)=-x^2-x-1</t>
-  </si>
-  <si>
-    <t>Representacion grafica de la función f(x)=-x^2-1</t>
-  </si>
-  <si>
-    <r>
-      <t>Representación gráfica de la función f(x)=-x</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>-x-2</t>
-    </r>
+    <t>Grafica de la funcion f(x)=6x</t>
+  </si>
+  <si>
+    <t>Grafica la la funcion f(x)=3x+4</t>
+  </si>
+  <si>
+    <t>Grafica de la funcion f(x)=-3x-2</t>
+  </si>
+  <si>
+    <t>Una grafica de una funcion polinomica con grado 4 similar a esta</t>
+  </si>
+  <si>
+    <t>Grafica de la función f(x)=x^2-3x+1, la gráfica con la etiqueta de la fórmula de la función.</t>
+  </si>
+  <si>
+    <t>Grafica de la función f(x)=-x^2+x+1, la gráfica con la etiqueta de la fórmula de la función.</t>
+  </si>
+  <si>
+    <t>Grafica de la función f(x)=x^2+x-1, la gráfica con la etiqueta de la fórmula de la función.</t>
+  </si>
+  <si>
+    <t>Representacion grafica de la funcion f(x)= 0.25x^6-1.5x^4+0.4x^2-0.45x-0.2</t>
+  </si>
+  <si>
+    <t>Realizar una grafica similar a esta</t>
+  </si>
+  <si>
+    <t>Grafica de la función f(x)=2x^5-5x^3-0.2x+1</t>
+  </si>
+  <si>
+    <t>Grafica de la funcion f(x)= 3x^3-2x+1</t>
+  </si>
+  <si>
+    <t>Una grafica de una funcion cubica  similar a esta, en la  gráfica se debe  escribir: a_3&lt;0.</t>
+  </si>
+  <si>
+    <t>Una grafica de una funcion cubica  similar a esta, en la  gráfica se debe  escribir: a_3&gt;0.</t>
+  </si>
+  <si>
+    <t>Una grafica como esta</t>
+  </si>
+  <si>
+    <t>Grafica de grado impar mayor que 5</t>
   </si>
 </sst>
 </file>
@@ -708,7 +628,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -855,19 +775,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -1613,6 +1520,10 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1696,10 +1607,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="51">
@@ -1833,6 +1740,528 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>2122714</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>843643</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>4332514</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>2638153</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="16124464" y="18805072"/>
+          <a:ext cx="2209800" cy="1794510"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1115786</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>530679</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>3325586</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>2325189</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15117536" y="24710572"/>
+          <a:ext cx="2209800" cy="1794510"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1020536</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>122465</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>3230336</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>1916975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15022286" y="27295929"/>
+          <a:ext cx="2209800" cy="1794510"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1115785</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>244929</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>3325585</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>2039439</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15117535" y="29377822"/>
+          <a:ext cx="2209800" cy="1794510"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1782536</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>312965</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>3992336</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>2107475</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagen 6"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15784286" y="31691036"/>
+          <a:ext cx="2209800" cy="1794510"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1279071</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>312964</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>3488871</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>2107474</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagen 7"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15280821" y="34562143"/>
+          <a:ext cx="2209800" cy="1794510"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1047750</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>204107</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>3257550</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>1998617</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagen 8"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15049500" y="36793714"/>
+          <a:ext cx="2209800" cy="1794510"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1564821</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>503464</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>3774621</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>2297974</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Imagen 9"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15566571" y="39338250"/>
+          <a:ext cx="2209800" cy="1794510"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>816429</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>312965</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>3026229</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>2107475</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Imagen 10"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="14818179" y="41828358"/>
+          <a:ext cx="2209800" cy="1794510"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>2286001</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>435429</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>4495801</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>2229939</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Imagen 11"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="16287751" y="44413715"/>
+          <a:ext cx="2209800" cy="1794510"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>816429</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>40821</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>3026229</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>1835331</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Imagen 12"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="14818179" y="47053500"/>
+          <a:ext cx="2209800" cy="1794510"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
@@ -2547,9 +2976,9 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P68"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J34" sqref="J34"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="140" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2587,14 +3016,14 @@
       <c r="B2" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="78" t="s">
+      <c r="C2" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="79"/>
-      <c r="F2" s="71" t="s">
+      <c r="D2" s="81"/>
+      <c r="F2" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="72"/>
+      <c r="G2" s="74"/>
       <c r="H2" s="42"/>
       <c r="I2" s="42"/>
       <c r="J2" s="16"/>
@@ -2604,12 +3033,12 @@
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="80">
+      <c r="C3" s="82">
         <v>11</v>
       </c>
-      <c r="D3" s="81"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="74"/>
+      <c r="D3" s="83"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="76"/>
       <c r="H3" s="42"/>
       <c r="I3" s="42"/>
       <c r="J3" s="16"/>
@@ -2619,10 +3048,10 @@
       <c r="B4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="80" t="s">
+      <c r="C4" s="82" t="s">
         <v>147</v>
       </c>
-      <c r="D4" s="81"/>
+      <c r="D4" s="83"/>
       <c r="E4" s="5"/>
       <c r="F4" s="41" t="s">
         <v>55</v>
@@ -2640,10 +3069,10 @@
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="82" t="s">
+      <c r="C5" s="84" t="s">
         <v>148</v>
       </c>
-      <c r="D5" s="83"/>
+      <c r="D5" s="85"/>
       <c r="E5" s="5"/>
       <c r="F5" s="39" t="str">
         <f>IF(G4="Recurso","Motor del recurso","")</f>
@@ -2676,7 +3105,7 @@
         <v>40</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D7" s="25" t="s">
         <v>39</v>
@@ -2694,12 +3123,12 @@
       <c r="C8" s="10"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
-      <c r="F8" s="75" t="s">
+      <c r="F8" s="77" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="76"/>
-      <c r="H8" s="76"/>
-      <c r="I8" s="77"/>
+      <c r="G8" s="78"/>
+      <c r="H8" s="78"/>
+      <c r="I8" s="79"/>
       <c r="J8" s="18"/>
       <c r="K8" s="12"/>
       <c r="L8" s="2"/>
@@ -2773,10 +3202,10 @@
         <v>MA_11_02_REC150_IMG01a.jpg</v>
       </c>
       <c r="I10" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="J10" s="67" t="s">
         <v>161</v>
-      </c>
-      <c r="J10" s="67" t="s">
-        <v>163</v>
       </c>
       <c r="K10" s="70"/>
     </row>
@@ -2788,7 +3217,7 @@
         <v>149</v>
       </c>
       <c r="C11" s="22" t="str">
-        <f t="shared" ref="C11:C19" si="1">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
+        <f>IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Recurso F13</v>
       </c>
       <c r="D11" s="14" t="s">
@@ -2798,7 +3227,7 @@
         <v>146</v>
       </c>
       <c r="F11" s="14" t="str">
-        <f t="shared" ref="F11:F19" si="2">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I11="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f>IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I11="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v>MA_11_02_REC150_IMG02n.jpg</v>
       </c>
       <c r="G11" s="14" t="str">
@@ -2806,14 +3235,14 @@
         <v>800 x 460 px</v>
       </c>
       <c r="H11" s="14" t="str">
-        <f t="shared" ref="H11:H19" si="3">IF(AND(I11&lt;&gt;"",I11&lt;&gt;0),IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f>IF(AND(I11&lt;&gt;"",I11&lt;&gt;0),IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v>MA_11_02_REC150_IMG02a.jpg</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J11" s="67" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="K11" s="70"/>
     </row>
@@ -2825,7 +3254,7 @@
         <v>149</v>
       </c>
       <c r="C12" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(OR(B12&lt;&gt;"",J12&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Recurso F13</v>
       </c>
       <c r="D12" s="14" t="s">
@@ -2835,7 +3264,7 @@
         <v>146</v>
       </c>
       <c r="F12" s="14" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(OR(B12&lt;&gt;"",J12&lt;&gt;""),CONCATENATE($C$7,"_",$A12,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I12="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v>MA_11_02_REC150_IMG03n.jpg</v>
       </c>
       <c r="G12" s="14" t="str">
@@ -2843,14 +3272,14 @@
         <v>800 x 460 px</v>
       </c>
       <c r="H12" s="14" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(AND(I12&lt;&gt;"",I12&lt;&gt;0),IF(OR(B12&lt;&gt;"",J12&lt;&gt;""),CONCATENATE($C$7,"_",$A12,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v>MA_11_02_REC150_IMG03a.jpg</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J12" s="67" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="K12" s="70"/>
     </row>
@@ -2861,9 +3290,9 @@
       <c r="B13" s="68" t="s">
         <v>149</v>
       </c>
-      <c r="C13" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>Recurso F13</v>
+      <c r="C13" s="22" t="e">
+        <f>IF(OR(B13&lt;&gt;"",#REF!&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
+        <v>#REF!</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>145</v>
@@ -2871,23 +3300,23 @@
       <c r="E13" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="F13" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>MA_11_02_REC150_IMG04n.jpg</v>
-      </c>
-      <c r="G13" s="14" t="str">
+      <c r="F13" s="14" t="e">
+        <f>IF(OR(B13&lt;&gt;"",#REF!&lt;&gt;""),CONCATENATE($C$7,"_",$A13,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I13="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G13" s="14" t="e">
         <f>IF(F13&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>800 x 460 px</v>
-      </c>
-      <c r="H13" s="14" t="str">
-        <f t="shared" si="3"/>
-        <v>MA_11_02_REC150_IMG04a.jpg</v>
+        <v>#REF!</v>
+      </c>
+      <c r="H13" s="14" t="e">
+        <f>IF(AND(I13&lt;&gt;"",I13&lt;&gt;0),IF(OR(B13&lt;&gt;"",#REF!&lt;&gt;""),CONCATENATE($C$7,"_",$A13,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <v>#REF!</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J13" s="67" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K13" s="70"/>
     </row>
@@ -2899,7 +3328,7 @@
         <v>149</v>
       </c>
       <c r="C14" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(OR(B14&lt;&gt;"",J13&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Recurso F13</v>
       </c>
       <c r="D14" s="14" t="s">
@@ -2909,7 +3338,7 @@
         <v>146</v>
       </c>
       <c r="F14" s="14" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(OR(B14&lt;&gt;"",J13&lt;&gt;""),CONCATENATE($C$7,"_",$A14,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I14="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v>MA_11_02_REC150_IMG05n.jpg</v>
       </c>
       <c r="G14" s="14" t="str">
@@ -2917,11 +3346,11 @@
         <v>800 x 460 px</v>
       </c>
       <c r="H14" s="14" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(AND(I14&lt;&gt;"",I14&lt;&gt;0),IF(OR(B14&lt;&gt;"",J13&lt;&gt;""),CONCATENATE($C$7,"_",$A14,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v>MA_11_02_REC150_IMG05a.jpg</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J14" s="67" t="s">
         <v>167</v>
@@ -2935,9 +3364,9 @@
       <c r="B15" s="68" t="s">
         <v>149</v>
       </c>
-      <c r="C15" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>Recurso F13</v>
+      <c r="C15" s="22" t="e">
+        <f>IF(OR(B15&lt;&gt;"",#REF!&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
+        <v>#REF!</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>145</v>
@@ -2945,23 +3374,23 @@
       <c r="E15" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="F15" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>MA_11_02_REC150_IMG06n.jpg</v>
-      </c>
-      <c r="G15" s="14" t="str">
+      <c r="F15" s="14" t="e">
+        <f>IF(OR(B15&lt;&gt;"",#REF!&lt;&gt;""),CONCATENATE($C$7,"_",$A15,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I15="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G15" s="14" t="e">
         <f>IF(F15&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>800 x 460 px</v>
-      </c>
-      <c r="H15" s="14" t="str">
-        <f t="shared" si="3"/>
-        <v>MA_11_02_REC150_IMG06a.jpg</v>
+        <v>#REF!</v>
+      </c>
+      <c r="H15" s="14" t="e">
+        <f>IF(AND(I15&lt;&gt;"",I15&lt;&gt;0),IF(OR(B15&lt;&gt;"",#REF!&lt;&gt;""),CONCATENATE($C$7,"_",$A15,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <v>#REF!</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J15" s="67" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="K15" s="70"/>
     </row>
@@ -2973,7 +3402,7 @@
         <v>149</v>
       </c>
       <c r="C16" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(OR(B16&lt;&gt;"",J15&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Recurso F13</v>
       </c>
       <c r="D16" s="14" t="s">
@@ -2983,7 +3412,7 @@
         <v>146</v>
       </c>
       <c r="F16" s="14" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(OR(B16&lt;&gt;"",J15&lt;&gt;""),CONCATENATE($C$7,"_",$A16,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I16="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v>MA_11_02_REC150_IMG07n.jpg</v>
       </c>
       <c r="G16" s="14" t="str">
@@ -2991,14 +3420,14 @@
         <v>800 x 460 px</v>
       </c>
       <c r="H16" s="14" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(AND(I16&lt;&gt;"",I16&lt;&gt;0),IF(OR(B16&lt;&gt;"",J15&lt;&gt;""),CONCATENATE($C$7,"_",$A16,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v>MA_11_02_REC150_IMG07a.jpg</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="J16" s="67" t="s">
-        <v>169</v>
+        <v>159</v>
+      </c>
+      <c r="J16" s="14" t="s">
+        <v>166</v>
       </c>
       <c r="K16" s="66"/>
     </row>
@@ -3010,7 +3439,7 @@
         <v>149</v>
       </c>
       <c r="C17" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="C13:C19" si="1">IF(OR(B17&lt;&gt;"",J17&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Recurso F13</v>
       </c>
       <c r="D17" s="14" t="s">
@@ -3020,7 +3449,7 @@
         <v>146</v>
       </c>
       <c r="F17" s="14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="F13:F19" si="2">IF(OR(B17&lt;&gt;"",J17&lt;&gt;""),CONCATENATE($C$7,"_",$A17,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I17="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v>MA_11_02_REC150_IMG08n.jpg</v>
       </c>
       <c r="G17" s="14" t="str">
@@ -3028,14 +3457,14 @@
         <v>800 x 460 px</v>
       </c>
       <c r="H17" s="14" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="H13:H19" si="3">IF(AND(I17&lt;&gt;"",I17&lt;&gt;0),IF(OR(B17&lt;&gt;"",J17&lt;&gt;""),CONCATENATE($C$7,"_",$A17,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v>MA_11_02_REC150_IMG08a.jpg</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J17" s="67" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K17" s="15"/>
     </row>
@@ -3069,16 +3498,16 @@
         <v>MA_11_02_REC150_IMG09a.jpg</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J18" s="67" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="K18" s="15"/>
     </row>
-    <row r="19" spans="1:11" s="12" customFormat="1" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="12" customFormat="1" ht="238.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B19" s="68" t="s">
         <v>149</v>
@@ -3106,18 +3535,16 @@
         <v>MA_11_02_REC150_IMG10a.jpg</v>
       </c>
       <c r="I19" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="J19" s="67" t="s">
-        <v>172</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="J19" s="67"/>
       <c r="K19" s="15" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="12" customFormat="1" ht="206.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
         <v>158</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" s="12" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
-        <v>159</v>
       </c>
       <c r="B20" s="68" t="s">
         <v>149</v>
@@ -3151,9 +3578,7 @@
       <c r="J20" s="67" t="s">
         <v>173</v>
       </c>
-      <c r="K20" s="15" t="s">
-        <v>160</v>
-      </c>
+      <c r="K20" s="15"/>
     </row>
     <row r="21" spans="1:11" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
@@ -3166,7 +3591,7 @@
       <c r="H21" s="14"/>
       <c r="I21" s="14"/>
       <c r="J21" s="67" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="K21" s="15"/>
     </row>
@@ -3180,8 +3605,8 @@
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
       <c r="I22" s="14"/>
-      <c r="J22" s="14" t="s">
-        <v>175</v>
+      <c r="J22" s="12" t="s">
+        <v>172</v>
       </c>
       <c r="K22" s="15"/>
     </row>
@@ -3195,12 +3620,12 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14"/>
-      <c r="J23" s="103" t="s">
-        <v>176</v>
+      <c r="J23" s="72" t="s">
+        <v>174</v>
       </c>
       <c r="K23" s="15"/>
     </row>
-    <row r="24" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="12" customFormat="1" ht="235.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
       <c r="B24" s="13"/>
       <c r="C24" s="13"/>
@@ -3210,12 +3635,12 @@
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
       <c r="I24" s="14"/>
-      <c r="J24" s="103" t="s">
-        <v>176</v>
-      </c>
-      <c r="K24" s="15"/>
-    </row>
-    <row r="25" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J24" s="72"/>
+      <c r="K24" s="15" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="12" customFormat="1" ht="153.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13"/>
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
@@ -3225,12 +3650,12 @@
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
       <c r="I25" s="14"/>
-      <c r="J25" s="103" t="s">
-        <v>177</v>
-      </c>
-      <c r="K25" s="15"/>
-    </row>
-    <row r="26" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J25" s="72"/>
+      <c r="K25" s="15" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="12" customFormat="1" ht="177" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13"/>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
@@ -3240,12 +3665,12 @@
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
       <c r="I26" s="14"/>
-      <c r="J26" s="103" t="s">
-        <v>178</v>
-      </c>
-      <c r="K26" s="15"/>
-    </row>
-    <row r="27" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J26" s="72"/>
+      <c r="K26" s="15" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" s="12" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
       <c r="B27" s="13"/>
       <c r="C27" s="13"/>
@@ -3255,10 +3680,10 @@
       <c r="G27" s="14"/>
       <c r="H27" s="14"/>
       <c r="I27" s="14"/>
-      <c r="J27" s="103" t="s">
-        <v>179</v>
-      </c>
-      <c r="K27" s="15"/>
+      <c r="J27" s="72"/>
+      <c r="K27" s="15" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="28" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
@@ -3271,11 +3696,11 @@
       <c r="H28" s="14"/>
       <c r="I28" s="14"/>
       <c r="J28" s="14" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="K28" s="15"/>
     </row>
-    <row r="29" spans="1:11" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
@@ -3285,12 +3710,12 @@
       <c r="G29" s="14"/>
       <c r="H29" s="14"/>
       <c r="I29" s="14"/>
-      <c r="J29" s="102" t="s">
-        <v>181</v>
+      <c r="J29" s="71" t="s">
+        <v>177</v>
       </c>
       <c r="K29" s="15"/>
     </row>
-    <row r="30" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" s="12" customFormat="1" ht="183.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
       <c r="C30" s="13"/>
@@ -3300,12 +3725,12 @@
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
       <c r="I30" s="14"/>
-      <c r="J30" s="103" t="s">
-        <v>182</v>
-      </c>
-      <c r="K30" s="15"/>
-    </row>
-    <row r="31" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J30" s="72"/>
+      <c r="K30" s="15" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" s="12" customFormat="1" ht="176.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
@@ -3315,12 +3740,12 @@
       <c r="G31" s="14"/>
       <c r="H31" s="14"/>
       <c r="I31" s="14"/>
-      <c r="J31" s="103" t="s">
-        <v>183</v>
-      </c>
-      <c r="K31" s="15"/>
-    </row>
-    <row r="32" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J31" s="72"/>
+      <c r="K31" s="15" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" s="12" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
       <c r="C32" s="13"/>
@@ -3330,12 +3755,12 @@
       <c r="G32" s="14"/>
       <c r="H32" s="14"/>
       <c r="I32" s="14"/>
-      <c r="J32" s="103" t="s">
-        <v>184</v>
-      </c>
-      <c r="K32" s="15"/>
-    </row>
-    <row r="33" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J32" s="72"/>
+      <c r="K32" s="15" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" s="12" customFormat="1" ht="194.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
       <c r="C33" s="13"/>
@@ -3345,12 +3770,12 @@
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
       <c r="I33" s="14"/>
-      <c r="J33" s="103" t="s">
-        <v>185</v>
-      </c>
-      <c r="K33" s="15"/>
-    </row>
-    <row r="34" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J33" s="72"/>
+      <c r="K33" s="15" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" s="12" customFormat="1" ht="239.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="B34" s="13"/>
       <c r="C34" s="13"/>
@@ -3360,12 +3785,10 @@
       <c r="G34" s="14"/>
       <c r="H34" s="14"/>
       <c r="I34" s="14"/>
-      <c r="J34" s="103" t="s">
-        <v>187</v>
-      </c>
+      <c r="J34" s="72"/>
       <c r="K34" s="15"/>
     </row>
-    <row r="35" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" s="12" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
       <c r="B35" s="13"/>
       <c r="C35" s="13"/>
@@ -3375,10 +3798,10 @@
       <c r="G35" s="14"/>
       <c r="H35" s="14"/>
       <c r="I35" s="14"/>
-      <c r="J35" s="103" t="s">
-        <v>186</v>
-      </c>
-      <c r="K35" s="15"/>
+      <c r="J35" s="72"/>
+      <c r="K35" s="15" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="36" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
@@ -3390,7 +3813,7 @@
       <c r="G36" s="14"/>
       <c r="H36" s="14"/>
       <c r="I36" s="14"/>
-      <c r="J36" s="102"/>
+      <c r="J36" s="71"/>
       <c r="K36" s="15"/>
     </row>
     <row r="37" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -3990,7 +4413,8 @@
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4020,25 +4444,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="88" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="88"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="90"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="33"/>
-      <c r="C2" s="89" t="s">
+      <c r="C2" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="90"/>
-      <c r="E2" s="91"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="93"/>
       <c r="F2" s="34"/>
     </row>
     <row r="3" spans="1:11" ht="63" x14ac:dyDescent="0.25">
@@ -4046,11 +4470,11 @@
         <v>43</v>
       </c>
       <c r="B3" s="33"/>
-      <c r="C3" s="95" t="s">
+      <c r="C3" s="97" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="96"/>
-      <c r="E3" s="97"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="99"/>
       <c r="F3" s="34"/>
       <c r="H3" s="24" t="s">
         <v>18</v>
@@ -4101,11 +4525,11 @@
       <c r="C5" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="98" t="str">
+      <c r="D5" s="100" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_CO")</f>
         <v>MA_11_02_CO</v>
       </c>
-      <c r="E5" s="99"/>
+      <c r="E5" s="101"/>
       <c r="F5" s="34"/>
       <c r="H5" s="24" t="s">
         <v>22</v>
@@ -4150,12 +4574,12 @@
       <c r="C7" s="64" t="s">
         <v>127</v>
       </c>
-      <c r="D7" s="84" t="str">
+      <c r="D7" s="86" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D5,".xls")</f>
         <v>SolicitudGrafica_MA_11_02_CO.xls</v>
       </c>
-      <c r="E7" s="84"/>
-      <c r="F7" s="85"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="87"/>
       <c r="H7" s="24" t="s">
         <v>24</v>
       </c>
@@ -4249,14 +4673,14 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="86" t="s">
+      <c r="A13" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="87"/>
-      <c r="C13" s="87"/>
-      <c r="D13" s="87"/>
-      <c r="E13" s="87"/>
-      <c r="F13" s="88"/>
+      <c r="B13" s="89"/>
+      <c r="C13" s="89"/>
+      <c r="D13" s="89"/>
+      <c r="E13" s="89"/>
+      <c r="F13" s="90"/>
       <c r="I13" s="24" t="s">
         <v>33</v>
       </c>
@@ -4289,12 +4713,12 @@
         <v>46</v>
       </c>
       <c r="B15" s="33"/>
-      <c r="C15" s="89" t="s">
+      <c r="C15" s="91" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="90"/>
-      <c r="E15" s="90"/>
-      <c r="F15" s="91"/>
+      <c r="D15" s="92"/>
+      <c r="E15" s="92"/>
+      <c r="F15" s="93"/>
       <c r="J15" s="24">
         <v>12</v>
       </c>
@@ -4334,12 +4758,12 @@
       <c r="C17" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="92" t="str">
+      <c r="D17" s="94" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_",K45)</f>
         <v>MA_11_02_REC130</v>
       </c>
-      <c r="E17" s="93"/>
-      <c r="F17" s="94"/>
+      <c r="E17" s="95"/>
+      <c r="F17" s="96"/>
       <c r="J17" s="24">
         <v>14</v>
       </c>
@@ -4355,12 +4779,12 @@
       <c r="C18" s="64" t="s">
         <v>128</v>
       </c>
-      <c r="D18" s="84" t="str">
+      <c r="D18" s="86" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D17,".xls")</f>
         <v>SolicitudGrafica_MA_11_02_REC130.xls</v>
       </c>
-      <c r="E18" s="84"/>
-      <c r="F18" s="85"/>
+      <c r="E18" s="86"/>
+      <c r="F18" s="87"/>
       <c r="J18" s="24">
         <v>15</v>
       </c>
@@ -4752,41 +5176,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="102" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="100" t="s">
+      <c r="B1" s="102" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="100" t="s">
+      <c r="C1" s="102" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="100" t="s">
+      <c r="D1" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="100" t="s">
+      <c r="E1" s="102" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="100" t="s">
+      <c r="F1" s="102" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="100" t="s">
+      <c r="G1" s="102" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="101" t="s">
+      <c r="H1" s="103" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="101"/>
-      <c r="J1" s="101"/>
+      <c r="I1" s="103"/>
+      <c r="J1" s="103"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="100"/>
-      <c r="B2" s="100"/>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
+      <c r="A2" s="102"/>
+      <c r="B2" s="102"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
       <c r="H2" s="43" t="s">
         <v>65</v>
       </c>

</xml_diff>